<commit_message>
antes de very positive e very negative addition
</commit_message>
<xml_diff>
--- a/TestResult.xlsx
+++ b/TestResult.xlsx
@@ -521,7 +521,7 @@
         <v>0.6310413597568404</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4723216039240778</v>
+        <v>0.4698579619822297</v>
       </c>
       <c r="J2" t="n">
         <v>0.8000857010145761</v>
@@ -594,10 +594,10 @@
         <v>0.12</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3365849853028059</v>
+        <v>1.222175083717947e-17</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4723216039240778</v>
+        <v>0.4698579619822297</v>
       </c>
       <c r="J4" t="n">
         <v>0.6936418300135643</v>
@@ -606,7 +606,7 @@
         <v>0.680884174355996</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2165849853028059</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="5">
@@ -670,10 +670,10 @@
         <v>0.5</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6354218043317128</v>
+        <v>0.6673333333333329</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2874308538537654</v>
+        <v>0.2085278213706131</v>
       </c>
       <c r="J6" t="n">
         <v>0.8336666666666664</v>
@@ -682,7 +682,7 @@
         <v>0.8919666127539357</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1354218043317128</v>
+        <v>0.1673333333333329</v>
       </c>
     </row>
     <row r="7">
@@ -711,7 +711,7 @@
         <v>0.6342816344660573</v>
       </c>
       <c r="I7" t="n">
-        <v>0.4599435772042542</v>
+        <v>0.4519274383469447</v>
       </c>
       <c r="J7" t="n">
         <v>0.1905605150983513</v>
@@ -822,10 +822,10 @@
         <v>0.85</v>
       </c>
       <c r="H10" t="n">
-        <v>0.5174572920123405</v>
+        <v>0.6673333333333329</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2778574283681999</v>
+        <v>0.1962864880001979</v>
       </c>
       <c r="J10" t="n">
         <v>0.6486161655729349</v>
@@ -834,7 +834,7 @@
         <v>0.7205936468619331</v>
       </c>
       <c r="L10" t="n">
-        <v>0.3325427079876595</v>
+        <v>0.1826666666666671</v>
       </c>
     </row>
     <row r="11">
@@ -860,10 +860,10 @@
         <v>0.85</v>
       </c>
       <c r="H11" t="n">
-        <v>0.667333332444444</v>
+        <v>0.6673333333333329</v>
       </c>
       <c r="I11" t="n">
-        <v>0.2640339039264897</v>
+        <v>0.1795051197566921</v>
       </c>
       <c r="J11" t="n">
         <v>0.4999999999999994</v>
@@ -872,7 +872,7 @@
         <v>0.5499998996992981</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1826666675555559</v>
+        <v>0.1826666666666671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate data from FS Sugeno
</commit_message>
<xml_diff>
--- a/TestResult.xlsx
+++ b/TestResult.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,25 +466,45 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>V_MemoryUsage</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>V_ProcessorLoad</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>V_InpNetThroughput</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>V_OutNetThroughput</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>V_OutBandwidth</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>V_Latency</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>CLPVariation</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>CLPVariation_pred</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Critical</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>FinalOut</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>erro_CLP</t>
         </is>
@@ -510,18 +530,30 @@
         <v>0.8</v>
       </c>
       <c r="G2" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="M2" t="n">
         <v>0.73</v>
       </c>
-      <c r="H2" t="n">
+      <c r="N2" t="n">
         <v>0.6562615384615386</v>
       </c>
-      <c r="I2" t="n">
-        <v>0.316923076923077</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.8280000000000001</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="O2" t="n">
         <v>0.07373846153846142</v>
       </c>
     </row>
@@ -545,18 +577,30 @@
         <v>0.53</v>
       </c>
       <c r="G3" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="M3" t="n">
         <v>-0.82</v>
       </c>
-      <c r="H3" t="n">
+      <c r="N3" t="n">
         <v>-0.8154180000000001</v>
       </c>
-      <c r="I3" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.03980000000000006</v>
-      </c>
-      <c r="K3" t="n">
+      <c r="O3" t="n">
         <v>0.004581999999999864</v>
       </c>
     </row>
@@ -580,18 +624,30 @@
         <v>0.4</v>
       </c>
       <c r="G4" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="M4" t="n">
         <v>0.12</v>
       </c>
-      <c r="H4" t="n">
+      <c r="N4" t="n">
         <v>0.02046153846153853</v>
       </c>
-      <c r="I4" t="n">
-        <v>0.316923076923077</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.08000000000000008</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="O4" t="n">
         <v>0.09953846153846146</v>
       </c>
     </row>
@@ -615,18 +671,30 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M5" t="n">
         <v>-0.85</v>
       </c>
-      <c r="H5" t="n">
+      <c r="N5" t="n">
         <v>-0.8200000000000001</v>
       </c>
-      <c r="I5" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
+      <c r="O5" t="n">
         <v>0.02999999999999992</v>
       </c>
     </row>
@@ -653,15 +721,27 @@
         <v>0.5</v>
       </c>
       <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
         <v>0.5532165841584158</v>
       </c>
-      <c r="I6" t="n">
-        <v>-0.5625</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.5299999999999998</v>
-      </c>
-      <c r="K6" t="n">
+      <c r="O6" t="n">
         <v>0.05321658415841579</v>
       </c>
     </row>
@@ -685,18 +765,30 @@
         <v>1</v>
       </c>
       <c r="G7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="M7" t="n">
         <v>0.8</v>
       </c>
-      <c r="H7" t="n">
+      <c r="N7" t="n">
         <v>0.8548214285714285</v>
       </c>
-      <c r="I7" t="n">
-        <v>-0.03214285714285708</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" t="n">
+      <c r="O7" t="n">
         <v>0.05482142857142847</v>
       </c>
     </row>
@@ -720,18 +812,30 @@
         <v>0.5</v>
       </c>
       <c r="G8" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="M8" t="n">
         <v>-0.31</v>
       </c>
-      <c r="H8" t="n">
+      <c r="N8" t="n">
         <v>-0.381205128205128</v>
       </c>
-      <c r="I8" t="n">
-        <v>0.6599999999999999</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="O8" t="n">
         <v>0.07120512820512803</v>
       </c>
     </row>
@@ -755,18 +859,30 @@
         <v>0.5</v>
       </c>
       <c r="G9" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="M9" t="n">
         <v>-0.65</v>
       </c>
-      <c r="H9" t="n">
+      <c r="N9" t="n">
         <v>-0.4980191939671157</v>
       </c>
-      <c r="I9" t="n">
-        <v>0.6599999999999999</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.01399999999999979</v>
-      </c>
-      <c r="K9" t="n">
+      <c r="O9" t="n">
         <v>0.1519808060328843</v>
       </c>
     </row>
@@ -790,18 +906,30 @@
         <v>0.5</v>
       </c>
       <c r="G10" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M10" t="n">
         <v>0.85</v>
       </c>
-      <c r="H10" t="n">
+      <c r="N10" t="n">
         <v>0.745345</v>
       </c>
-      <c r="I10" t="n">
-        <v>-0.7975</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.2179999999999999</v>
-      </c>
-      <c r="K10" t="n">
+      <c r="O10" t="n">
         <v>0.1046549999999999</v>
       </c>
     </row>
@@ -825,18 +953,30 @@
         <v>0.6</v>
       </c>
       <c r="G11" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="M11" t="n">
         <v>0.85</v>
       </c>
-      <c r="H11" t="n">
+      <c r="N11" t="n">
         <v>0.9317500000000001</v>
       </c>
-      <c r="I11" t="n">
-        <v>-0.925</v>
-      </c>
-      <c r="J11" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" t="n">
+      <c r="O11" t="n">
         <v>0.0817500000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
identaçao, comentários, novas MF simétricas
</commit_message>
<xml_diff>
--- a/TestResult.xlsx
+++ b/TestResult.xlsx
@@ -551,10 +551,10 @@
         <v>0.73</v>
       </c>
       <c r="N2" t="n">
-        <v>0.6562615384615386</v>
+        <v>0.6562615384615387</v>
       </c>
       <c r="O2" t="n">
-        <v>0.07373846153846142</v>
+        <v>0.07373846153846131</v>
       </c>
     </row>
     <row r="3">
@@ -598,10 +598,10 @@
         <v>-0.82</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.8154180000000001</v>
+        <v>-0.8105953846153846</v>
       </c>
       <c r="O3" t="n">
-        <v>0.004581999999999864</v>
+        <v>0.009404615384615345</v>
       </c>
     </row>
     <row r="4">
@@ -645,10 +645,10 @@
         <v>0.12</v>
       </c>
       <c r="N4" t="n">
-        <v>0.02046153846153853</v>
+        <v>0.02046153846153852</v>
       </c>
       <c r="O4" t="n">
-        <v>0.09953846153846146</v>
+        <v>0.09953846153846148</v>
       </c>
     </row>
     <row r="5">
@@ -739,10 +739,10 @@
         <v>0.5</v>
       </c>
       <c r="N6" t="n">
-        <v>0.5532165841584158</v>
+        <v>0.5500416666666665</v>
       </c>
       <c r="O6" t="n">
-        <v>0.05321658415841579</v>
+        <v>0.05004166666666654</v>
       </c>
     </row>
     <row r="7">
@@ -880,10 +880,10 @@
         <v>-0.65</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.4980191939671157</v>
+        <v>-0.5399939130434782</v>
       </c>
       <c r="O9" t="n">
-        <v>0.1519808060328843</v>
+        <v>0.1100060869565218</v>
       </c>
     </row>
     <row r="10">
@@ -974,10 +974,10 @@
         <v>0.85</v>
       </c>
       <c r="N11" t="n">
-        <v>0.9317500000000001</v>
+        <v>0.9070000000000001</v>
       </c>
       <c r="O11" t="n">
-        <v>0.0817500000000001</v>
+        <v>0.05700000000000016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>